<commit_message>
Organizador de Declaração de Imposto de Renda
Organizador de Declaração de imposto de renda afim de ajuda na organização dos dados do contribuinte
</commit_message>
<xml_diff>
--- a/Organizador de Declaração de Imposto de Renda.xlsx
+++ b/Organizador de Declaração de Imposto de Renda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/765d3175cee334b6/Área de Trabalho/Bootcamp Excel Santander DIO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="664" documentId="8_{947D5AB5-3FB9-422F-92FC-0AE3FADCF00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E66D6E4A-3FD7-431C-8C54-CE08F8336A47}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="14_{A6C74153-3716-47E3-AF7A-75E19A3D31AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EA88109-57A9-4643-9257-AEB6FDA43800}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="38616" windowHeight="15696" tabRatio="388" xr2:uid="{5DC14D9C-B3C1-4AFA-AAE2-90558E5CC0A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="388" activeTab="1" xr2:uid="{5DC14D9C-B3C1-4AFA-AAE2-90558E5CC0A4}"/>
   </bookViews>
   <sheets>
     <sheet name="TITULAR" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
   <si>
     <t>NOME</t>
   </si>
@@ -92,27 +92,9 @@
     <t>NÃO</t>
   </si>
   <si>
-    <t>JÔNATAS DAMASCENO DO NASCIMENTO</t>
-  </si>
-  <si>
-    <t>JONTPS@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>8697-745</t>
-  </si>
-  <si>
-    <t>TRAUMATURGO FERNANDES  R, - N°255</t>
-  </si>
-  <si>
-    <t>CHELLA</t>
-  </si>
-  <si>
     <t>PRÓXIMO -&gt;</t>
   </si>
   <si>
-    <t>1. Informes de Rendimento Bancário</t>
-  </si>
-  <si>
     <t>BANCO</t>
   </si>
   <si>
@@ -309,6 +291,27 @@
   </si>
   <si>
     <t>HOLERITE</t>
+  </si>
+  <si>
+    <t>CNPJ</t>
+  </si>
+  <si>
+    <t>Afonso yot gauset</t>
+  </si>
+  <si>
+    <t>Joana</t>
+  </si>
+  <si>
+    <t>Treze de março - N°26</t>
+  </si>
+  <si>
+    <t>Afonso.Yt@Hotmail.com</t>
+  </si>
+  <si>
+    <t>2. Informes de Rendimento Bancário</t>
+  </si>
+  <si>
+    <t>FREELANCE</t>
   </si>
 </sst>
 </file>
@@ -316,11 +319,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="169" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
-    <numFmt numFmtId="170" formatCode="00000\-000"/>
-    <numFmt numFmtId="173" formatCode="&quot;(&quot;00&quot;)&quot;00000&quot;-&quot;0000"/>
-    <numFmt numFmtId="174" formatCode="&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="177" formatCode="mmmm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
+    <numFmt numFmtId="165" formatCode="00000\-000"/>
+    <numFmt numFmtId="166" formatCode="&quot;(&quot;00&quot;)&quot;00000&quot;-&quot;0000"/>
+    <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="168" formatCode="mmmm\-yyyy"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -546,7 +549,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -556,7 +559,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -570,23 +572,14 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -603,14 +596,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -622,11 +615,11 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -638,23 +631,32 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="174" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -678,6 +680,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -693,7 +696,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="174" formatCode="&quot;R$&quot;\ #,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3573,13 +3575,17 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7FBA1E40-E657-43E2-AFCD-B6517923C32A}" name="Tabela2" displayName="Tabela2" ref="C8:E41" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7FBA1E40-E657-43E2-AFCD-B6517923C32A}" name="Tabela2" displayName="Tabela2" ref="C8:E41" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="C8:E41" xr:uid="{7FBA1E40-E657-43E2-AFCD-B6517923C32A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0C0F9232-7CD0-4CF7-9FB2-6923BE5FB3EE}" name="DATA " dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{748B31F2-E2AA-4426-87A1-427A7428F6A7}" name="CATEGORIA" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{22CD69CA-7D4A-4F9F-A16C-22168361B5C0}" name="VALOR" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{0C0F9232-7CD0-4CF7-9FB2-6923BE5FB3EE}" name="DATA " dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{748B31F2-E2AA-4426-87A1-427A7428F6A7}" name="CATEGORIA" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{22CD69CA-7D4A-4F9F-A16C-22168361B5C0}" name="VALOR" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3903,298 +3909,297 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85473FB-B12D-4272-B1C2-1101AF58058F}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1"/>
-    <col min="4" max="4" width="42.44140625" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" ht="22.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="C7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>53684249963</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="C8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="25">
+        <v>33554</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="C9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="C12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="27">
+        <v>8642832</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="28">
+        <v>11998654232</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="C14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="28">
+        <v>11998654232</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="C15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="C16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5"/>
+      <c r="C17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="C18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="2"/>
-      <c r="C7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="28">
-        <v>78596375263</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="2"/>
-      <c r="C8" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="29">
-        <v>34833</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="1"/>
-      <c r="C9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="1"/>
-      <c r="C10" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="1"/>
-      <c r="C11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="1"/>
-      <c r="C12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="1"/>
-      <c r="C13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="32">
-        <v>85997841456</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="1"/>
-      <c r="C14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="32">
-        <v>85997841456</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="1"/>
-      <c r="C15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="1"/>
-      <c r="C16" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="6"/>
-      <c r="C17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="1"/>
-      <c r="C18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="17.399999999999999" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="1"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A20" s="1"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="C4:D4"/>
   </mergeCells>
@@ -4204,7 +4209,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1" xr:uid="{B1DD2EF9-2665-4E9F-9101-536C74C9FFA4}"/>
+    <hyperlink ref="D15" r:id="rId1" display="JONTPS@GMAIL.COM" xr:uid="{B1DD2EF9-2665-4E9F-9101-536C74C9FFA4}"/>
     <hyperlink ref="D20" location="INFORMES!A1" display="PRÓXIMO -&gt;" xr:uid="{6BB91174-68D3-4431-886E-430FC1A4E8C7}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -4215,225 +4220,224 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A008FA-13A4-4AE9-81F0-0380C9CFC554}">
   <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:D22"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1"/>
-    <col min="4" max="4" width="42.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="C3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" ht="22.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="11"/>
+    </row>
+    <row r="4" spans="1:4" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.45">
+      <c r="D4" s="36"/>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="C6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="C7" s="16">
+      <c r="C7" s="38">
         <f>SUM(D11,D16,D21)</f>
-        <v>47920000</v>
-      </c>
-      <c r="D7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>47850000</v>
+      </c>
+      <c r="D7" s="38"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="C9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="C10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
-      <c r="C11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="35">
+      <c r="C11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="31">
         <v>500000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
-      <c r="C12" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="D13" s="36"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="32"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="C14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="15" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>74</v>
+      </c>
+      <c r="D14" s="32"/>
+    </row>
+    <row r="15" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="C15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
-      <c r="C16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="35">
-        <v>420000</v>
-      </c>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="31">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
-      <c r="C17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="D18" s="36"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="36"/>
-    </row>
-    <row r="20" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
-      <c r="C20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="C21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="35">
+      <c r="C21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="31">
         <v>47000000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
-      <c r="C22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
   </sheetData>
@@ -4462,274 +4466,345 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212F122D-048F-46E6-972A-5DE6A6F95014}">
   <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:6" ht="22.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="C4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="C8" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="C9" s="33">
+        <v>45775</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="22">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="C10" s="33">
+        <v>45776</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:9" ht="22.05" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="C4" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-    </row>
-    <row r="5" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="19"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="C8" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A9" s="1"/>
-      <c r="C9" s="37">
-        <v>45775</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="26">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="A10" s="1"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="E10" s="35">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C11" s="33">
+        <v>45777</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="35">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C12" s="33">
+        <v>45778</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C13" s="33">
+        <v>45779</v>
+      </c>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C14" s="33">
+        <v>45780</v>
+      </c>
+      <c r="D14" s="34"/>
+      <c r="E14" s="35"/>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C15" s="33">
+        <v>45781</v>
+      </c>
+      <c r="D15" s="34"/>
+      <c r="E15" s="35"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C16" s="33">
+        <v>45782</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
-    </row>
-    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C17" s="33">
+        <v>45783</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-    </row>
-    <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C18" s="33">
+        <v>45784</v>
+      </c>
+      <c r="D18" s="34"/>
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-    </row>
-    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C19" s="33">
+        <v>45785</v>
+      </c>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-    </row>
-    <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C20" s="33">
+        <v>45786</v>
+      </c>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C21" s="33">
+        <v>45787</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="35"/>
+    </row>
+    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-    </row>
-    <row r="23" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C22" s="33">
+        <v>45788</v>
+      </c>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+    </row>
+    <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39"/>
-    </row>
-    <row r="24" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C23" s="33">
+        <v>45789</v>
+      </c>
+      <c r="D23" s="34"/>
+      <c r="E23" s="35"/>
+    </row>
+    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
-    </row>
-    <row r="25" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C24" s="33">
+        <v>45790</v>
+      </c>
+      <c r="D24" s="34"/>
+      <c r="E24" s="35"/>
+    </row>
+    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="39"/>
-    </row>
-    <row r="26" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C25" s="33">
+        <v>45791</v>
+      </c>
+      <c r="D25" s="34"/>
+      <c r="E25" s="35"/>
+    </row>
+    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-    </row>
-    <row r="27" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C26" s="33">
+        <v>45792</v>
+      </c>
+      <c r="D26" s="34"/>
+      <c r="E26" s="35"/>
+    </row>
+    <row r="27" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="39"/>
-    </row>
-    <row r="28" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C27" s="33">
+        <v>45793</v>
+      </c>
+      <c r="D27" s="34"/>
+      <c r="E27" s="35"/>
+    </row>
+    <row r="28" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
-    </row>
-    <row r="29" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C28" s="33">
+        <v>45794</v>
+      </c>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
+    </row>
+    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="39"/>
-    </row>
-    <row r="30" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C29" s="33">
+        <v>45795</v>
+      </c>
+      <c r="D29" s="34"/>
+      <c r="E29" s="35"/>
+    </row>
+    <row r="30" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="39"/>
-    </row>
-    <row r="31" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C30" s="33">
+        <v>45796</v>
+      </c>
+      <c r="D30" s="34"/>
+      <c r="E30" s="35"/>
+    </row>
+    <row r="31" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="39"/>
-    </row>
-    <row r="32" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C31" s="33">
+        <v>45797</v>
+      </c>
+      <c r="D31" s="34"/>
+      <c r="E31" s="35"/>
+    </row>
+    <row r="32" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="39"/>
-    </row>
-    <row r="33" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C32" s="33">
+        <v>45798</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="39"/>
-    </row>
-    <row r="34" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C33" s="33">
+        <v>45799</v>
+      </c>
+      <c r="D33" s="34"/>
+      <c r="E33" s="35"/>
+    </row>
+    <row r="34" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
-    </row>
-    <row r="35" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C34" s="33">
+        <v>45800</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="35"/>
+    </row>
+    <row r="35" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
-    </row>
-    <row r="36" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C35" s="33">
+        <v>45801</v>
+      </c>
+      <c r="D35" s="34"/>
+      <c r="E35" s="35"/>
+    </row>
+    <row r="36" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="39"/>
-    </row>
-    <row r="37" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C36" s="33">
+        <v>45802</v>
+      </c>
+      <c r="D36" s="34"/>
+      <c r="E36" s="35"/>
+    </row>
+    <row r="37" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="39"/>
-    </row>
-    <row r="38" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C37" s="33">
+        <v>45803</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
+    </row>
+    <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="39"/>
-    </row>
-    <row r="39" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C38" s="33">
+        <v>45804</v>
+      </c>
+      <c r="D38" s="34"/>
+      <c r="E38" s="35"/>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="39"/>
-    </row>
-    <row r="40" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C39" s="33">
+        <v>45805</v>
+      </c>
+      <c r="D39" s="34"/>
+      <c r="E39" s="35"/>
+    </row>
+    <row r="40" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="39"/>
-    </row>
-    <row r="41" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C40" s="33">
+        <v>45806</v>
+      </c>
+      <c r="D40" s="34"/>
+      <c r="E40" s="35"/>
+    </row>
+    <row r="41" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="39"/>
+      <c r="C41" s="33">
+        <v>45807</v>
+      </c>
+      <c r="D41" s="34"/>
+      <c r="E41" s="35"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
@@ -4752,264 +4827,264 @@
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>